<commit_message>
Change PowerLinearity to IlluminationLinearity
</commit_message>
<xml_diff>
--- a/Tier System/in progress/v02-00/4DN-Metadata Tier System_2021-02-01_v02-00.xlsx
+++ b/Tier System/in progress/v02-00/4DN-Metadata Tier System_2021-02-01_v02-00.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/strambc/Documents/GitHub/MicroscopyMetadata4DNGuidelines_GitHub repo/Tier System/in progress/v02-00/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA96B87-B010-D74C-BB44-4609BC6AF744}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B316FEC-2702-4447-AE87-F64E18217E1D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28320" windowHeight="16740" tabRatio="914" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28320" windowHeight="16740" tabRatio="914" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tier system_v02-00" sheetId="12" r:id="rId1"/>
@@ -18,9 +18,9 @@
     <sheet name="Tier system_v02-00 MINIMAL" sheetId="14" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tier system_v02-00'!$A$2:$L$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Tier system_v02-00 MINIMAL'!$A$1:$H$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Tier system_v02-00 SUMMARY'!$A$2:$J$5</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tier system_v02-00'!$A$2:$I$5</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Tier system_v02-00 MINIMAL'!$A$2:$H$5</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Tier system_v02-00 SUMMARY'!$A$1:$J$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="50">
   <si>
     <t>-- required metadata --</t>
   </si>
@@ -377,7 +377,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -523,30 +523,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -653,6 +629,21 @@
         <color auto="1"/>
       </right>
       <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
       <bottom style="double">
         <color indexed="64"/>
       </bottom>
@@ -696,7 +687,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -783,40 +774,28 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -825,10 +804,10 @@
     <xf numFmtId="0" fontId="19" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -849,11 +828,62 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -867,12 +897,12 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -888,69 +918,11 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="35">
@@ -1341,8 +1313,8 @@
   </sheetPr>
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="45" zoomScaleNormal="53" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScale="45" zoomScaleNormal="53" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="29" x14ac:dyDescent="0.35"/>
@@ -1353,188 +1325,188 @@
     <col min="4" max="4" width="48" style="13" customWidth="1"/>
     <col min="5" max="5" width="54.5" style="13" customWidth="1"/>
     <col min="6" max="6" width="33" style="13" customWidth="1"/>
-    <col min="7" max="9" width="23.6640625" style="13" customWidth="1"/>
-    <col min="10" max="10" width="39.6640625" style="14" customWidth="1"/>
-    <col min="11" max="11" width="71.5" style="14" customWidth="1"/>
-    <col min="12" max="12" width="71.5" style="13" customWidth="1"/>
+    <col min="7" max="7" width="39.6640625" style="14" customWidth="1"/>
+    <col min="8" max="8" width="71.5" style="14" customWidth="1"/>
+    <col min="9" max="9" width="71.5" style="13" customWidth="1"/>
+    <col min="10" max="12" width="23.6640625" style="13" customWidth="1"/>
     <col min="13" max="16384" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="47" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="86" t="s">
+      <c r="B1" s="63"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
     </row>
     <row r="2" spans="1:13" s="23" customFormat="1" ht="80" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="81" t="s">
+      <c r="C2" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="82" t="s">
+      <c r="D2" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="82" t="s">
+      <c r="E2" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="82" t="s">
+      <c r="F2" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="82" t="s">
+      <c r="G2" s="62" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="62" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="82" t="s">
+      <c r="K2" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="82" t="s">
+      <c r="L2" s="62" t="s">
         <v>9</v>
-      </c>
-      <c r="J2" s="82" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="82" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="82" t="s">
-        <v>11</v>
       </c>
       <c r="M2" s="22"/>
     </row>
     <row r="3" spans="1:13" s="9" customFormat="1" ht="343" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="34">
+      <c r="B3" s="31">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="44" t="s">
+      <c r="G3" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="58" t="s">
+      <c r="K3" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="59"/>
-      <c r="J3" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" s="45" t="s">
-        <v>37</v>
-      </c>
+      <c r="L3" s="72"/>
       <c r="M3" s="12"/>
     </row>
     <row r="4" spans="1:13" s="10" customFormat="1" ht="406" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="67" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="29">
         <v>2</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="46" t="s">
+      <c r="E4" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="46" t="s">
+      <c r="F4" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="46" t="s">
+      <c r="G4" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="60" t="s">
+      <c r="K4" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="61"/>
-      <c r="J4" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="L4" s="49" t="s">
-        <v>38</v>
-      </c>
+      <c r="L4" s="74"/>
       <c r="M4" s="6"/>
     </row>
     <row r="5" spans="1:13" s="11" customFormat="1" ht="343" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="55"/>
+      <c r="A5" s="68"/>
       <c r="B5" s="17">
         <v>3</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="50" t="s">
+      <c r="D5" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="50" t="s">
+      <c r="E5" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="50" t="s">
+      <c r="F5" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="51" t="s">
+      <c r="G5" s="69" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="69"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="57" t="s">
+      <c r="K5" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="62"/>
-      <c r="J5" s="56" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="56"/>
-      <c r="L5" s="57"/>
+      <c r="L5" s="75"/>
       <c r="M5" s="7"/>
     </row>
     <row r="6" spans="1:13" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="2"/>
       <c r="C6" s="5"/>
       <c r="D6" s="15"/>
-      <c r="L6" s="16"/>
+      <c r="I6" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A4:A5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="24" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1549,100 +1521,107 @@
   </sheetPr>
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView zoomScale="58" zoomScaleNormal="89" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:J4"/>
+    <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="89" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="29" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.5" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="1" customWidth="1"/>
     <col min="3" max="3" width="35.5" style="4" customWidth="1"/>
     <col min="4" max="4" width="48" style="13" customWidth="1"/>
     <col min="5" max="5" width="54.5" style="13" customWidth="1"/>
     <col min="6" max="6" width="33" style="13" customWidth="1"/>
-    <col min="7" max="7" width="30.1640625" style="13" customWidth="1"/>
-    <col min="8" max="8" width="39.6640625" style="14" customWidth="1"/>
-    <col min="9" max="9" width="63.5" style="14" customWidth="1"/>
-    <col min="10" max="10" width="63.5" style="13" customWidth="1"/>
+    <col min="7" max="7" width="39.6640625" style="14" customWidth="1"/>
+    <col min="8" max="8" width="63.5" style="14" customWidth="1"/>
+    <col min="9" max="9" width="63.5" style="13" customWidth="1"/>
+    <col min="10" max="10" width="36.1640625" style="13" customWidth="1"/>
     <col min="11" max="16384" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="H1" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
+    <row r="1" spans="1:11" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="78" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
     </row>
     <row r="2" spans="1:11" s="23" customFormat="1" ht="80" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="58" t="s">
         <v>15</v>
-      </c>
-      <c r="H2" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="32" t="s">
-        <v>11</v>
       </c>
       <c r="K2" s="22"/>
     </row>
-    <row r="3" spans="1:11" s="9" customFormat="1" ht="207" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+    <row r="3" spans="1:11" s="9" customFormat="1" ht="272" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="37">
+      <c r="B3" s="33">
         <v>1</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="52" t="s">
+      <c r="F3" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="39" t="s">
+      <c r="G3" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="35" t="s">
         <v>29</v>
-      </c>
-      <c r="H3" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="40" t="s">
-        <v>37</v>
       </c>
       <c r="K3" s="12"/>
     </row>
-    <row r="4" spans="1:11" s="10" customFormat="1" ht="311" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="54" t="s">
+    <row r="4" spans="1:11" s="10" customFormat="1" ht="359" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="67" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="29">
@@ -1660,22 +1639,22 @@
       <c r="F4" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="21" t="s">
         <v>30</v>
-      </c>
-      <c r="H4" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="J4" s="27" t="s">
-        <v>38</v>
       </c>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" s="11" customFormat="1" ht="198" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="55"/>
+    <row r="5" spans="1:11" s="11" customFormat="1" ht="252" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="68"/>
       <c r="B5" s="17">
         <v>3</v>
       </c>
@@ -1691,30 +1670,30 @@
       <c r="F5" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="76"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" s="63"/>
-      <c r="J5" s="64"/>
       <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="2"/>
       <c r="C6" s="5"/>
       <c r="D6" s="15"/>
-      <c r="J6" s="16"/>
+      <c r="I6" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="H1:J1"/>
     <mergeCell ref="A4:A5"/>
-    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="43" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="28" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
 </file>
 
@@ -1724,9 +1703,9 @@
     <tabColor theme="8" tint="0.79998168889431442"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A2:I6"/>
   <sheetViews>
-    <sheetView zoomScale="72" zoomScaleNormal="72" zoomScalePageLayoutView="50" workbookViewId="0">
+    <sheetView zoomScale="56" zoomScaleNormal="72" zoomScalePageLayoutView="50" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -1743,72 +1722,60 @@
     <col min="9" max="16384" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="75" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="78"/>
-    </row>
     <row r="2" spans="1:9" s="23" customFormat="1" ht="107" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="74" t="s">
+      <c r="D2" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="74" t="s">
+      <c r="E2" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="74" t="s">
+      <c r="F2" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="74" t="s">
+      <c r="G2" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="74" t="s">
+      <c r="H2" s="58" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="9" customFormat="1" ht="242" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="37">
+      <c r="B3" s="33">
         <v>1</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="65" t="s">
+      <c r="F3" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="65" t="s">
+      <c r="G3" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="65" t="s">
+      <c r="H3" s="49" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="10" customFormat="1" ht="370" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="67" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="29">
@@ -1817,43 +1784,43 @@
       <c r="C4" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="68" t="s">
+      <c r="D4" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="68" t="s">
+      <c r="E4" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="68" t="s">
+      <c r="F4" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="66" t="s">
+      <c r="G4" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="66" t="s">
+      <c r="H4" s="50" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="11" customFormat="1" ht="158" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="55"/>
+      <c r="A5" s="68"/>
       <c r="B5" s="17">
         <v>3</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="69" t="s">
+      <c r="D5" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="69" t="s">
+      <c r="E5" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="69" t="s">
+      <c r="F5" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="67" t="s">
+      <c r="G5" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="70" t="s">
+      <c r="H5" s="54" t="s">
         <v>31</v>
       </c>
       <c r="I5"/>

</xml_diff>